<commit_message>
update tables for slides
</commit_message>
<xml_diff>
--- a/graphs_for_presentation/styled_tables/AttritionAnalysisTable.xlsx
+++ b/graphs_for_presentation/styled_tables/AttritionAnalysisTable.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amstone326/dimagi/deltacs-data-blog/graphs_for_presentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amstone326/dimagi/deltacs-data-blog/graphs_for_presentation/styled_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Bucket #</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>N (# of projects started at least 24 months ago)</t>
+  </si>
+  <si>
+    <t>Best connectivity (lowest 10% median DeltaCS)</t>
+  </si>
+  <si>
+    <t>Worst connectivity (highest 10% median DeltaCS)</t>
   </si>
 </sst>
 </file>
@@ -193,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -231,6 +237,11 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,16 +524,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:I8"/>
+  <dimension ref="D4:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="163" zoomScalePageLayoutView="163" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="3.83203125" style="1" customWidth="1"/>
@@ -555,14 +566,14 @@
       <c r="E5" s="7">
         <v>87</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="18">
         <v>0.874</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="13">
         <v>29</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="19">
         <v>0.621</v>
       </c>
     </row>
@@ -609,14 +620,66 @@
       <c r="E8" s="7">
         <v>88</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="18">
         <v>0.94299999999999995</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="13">
         <v>70</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="19">
+        <v>0.68600000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="D11" s="17"/>
+      <c r="E11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="D12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="7">
+        <v>35</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="13">
+        <v>10</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="D13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="7">
+        <v>35</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="13">
+        <v>29</v>
+      </c>
+      <c r="I13" s="8">
         <v>0.68600000000000005</v>
       </c>
     </row>

</xml_diff>